<commit_message>
Actualización del Sprint Backlog 2
</commit_message>
<xml_diff>
--- a/Desarrollo/Edutec/Gestión/Sprint 1/Sprint Backlog 1.xlsx
+++ b/Desarrollo/Edutec/Gestión/Sprint 1/Sprint Backlog 1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\Universidad\Edutec\Desarrollo\Edutec\Gestión\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\Universidad\Edutec\Desarrollo\Edutec\Gestión\Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73EEA103-18DD-40A7-B528-AB10B88DB8EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7E7DF7-D53E-4BB6-ABCF-281970C30E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -961,9 +961,6 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1054,13 +1051,19 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1070,12 +1073,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1085,6 +1082,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1303,7 +1303,7 @@
   <dimension ref="A1:Z1005"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -1636,17 +1636,17 @@
       <c r="Z10" s="3"/>
     </row>
     <row r="11" spans="1:26" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A11" s="99" t="s">
+      <c r="A11" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="100"/>
-      <c r="C11" s="100"/>
-      <c r="D11" s="100"/>
-      <c r="E11" s="100"/>
-      <c r="F11" s="100"/>
-      <c r="G11" s="100"/>
-      <c r="H11" s="100"/>
-      <c r="I11" s="101"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="91"/>
+      <c r="D11" s="91"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="91"/>
+      <c r="G11" s="91"/>
+      <c r="H11" s="91"/>
+      <c r="I11" s="92"/>
       <c r="J11" s="3"/>
       <c r="K11" s="12"/>
       <c r="L11" s="3"/>
@@ -2218,7 +2218,7 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A24" s="90"/>
+      <c r="A24" s="89"/>
       <c r="B24" s="37" t="s">
         <v>20</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>8</v>
       </c>
       <c r="I25" s="38" t="s">
-        <v>82</v>
+        <v>122</v>
       </c>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -2563,7 +2563,7 @@
         <v>12</v>
       </c>
       <c r="I31" s="47" t="s">
-        <v>24</v>
+        <v>122</v>
       </c>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
@@ -2608,26 +2608,26 @@
       <c r="H32" s="55">
         <v>4</v>
       </c>
-      <c r="I32" s="56" t="s">
-        <v>24</v>
-      </c>
-      <c r="J32" s="57"/>
-      <c r="K32" s="57"/>
-      <c r="L32" s="57"/>
-      <c r="M32" s="57"/>
-      <c r="N32" s="57"/>
-      <c r="O32" s="57"/>
-      <c r="P32" s="57"/>
-      <c r="Q32" s="57"/>
-      <c r="R32" s="57"/>
-      <c r="S32" s="57"/>
-      <c r="T32" s="57"/>
-      <c r="U32" s="57"/>
-      <c r="V32" s="57"/>
-      <c r="W32" s="57"/>
-      <c r="X32" s="57"/>
-      <c r="Y32" s="57"/>
-      <c r="Z32" s="57"/>
+      <c r="I32" s="107" t="s">
+        <v>122</v>
+      </c>
+      <c r="J32" s="56"/>
+      <c r="K32" s="56"/>
+      <c r="L32" s="56"/>
+      <c r="M32" s="56"/>
+      <c r="N32" s="56"/>
+      <c r="O32" s="56"/>
+      <c r="P32" s="56"/>
+      <c r="Q32" s="56"/>
+      <c r="R32" s="56"/>
+      <c r="S32" s="56"/>
+      <c r="T32" s="56"/>
+      <c r="U32" s="56"/>
+      <c r="V32" s="56"/>
+      <c r="W32" s="56"/>
+      <c r="X32" s="56"/>
+      <c r="Y32" s="56"/>
+      <c r="Z32" s="56"/>
     </row>
     <row r="33" spans="1:26" ht="17.25" customHeight="1">
       <c r="A33" s="40" t="s">
@@ -2836,12 +2836,12 @@
       <c r="Z38" s="3"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A39" s="93" t="s">
+      <c r="A39" s="97" t="s">
         <v>54</v>
       </c>
-      <c r="B39" s="94"/>
-      <c r="C39" s="94"/>
-      <c r="D39" s="95"/>
+      <c r="B39" s="98"/>
+      <c r="C39" s="98"/>
+      <c r="D39" s="94"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
@@ -2866,14 +2866,14 @@
       <c r="Z39" s="3"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A40" s="102" t="s">
+      <c r="A40" s="93" t="s">
         <v>55</v>
       </c>
-      <c r="B40" s="95"/>
-      <c r="C40" s="85" t="s">
+      <c r="B40" s="94"/>
+      <c r="C40" s="84" t="s">
         <v>114</v>
       </c>
-      <c r="D40" s="86" t="s">
+      <c r="D40" s="85" t="s">
         <v>57</v>
       </c>
       <c r="E40" s="3"/>
@@ -2900,14 +2900,14 @@
       <c r="Z40" s="3"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A41" s="91" t="s">
+      <c r="A41" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="B41" s="92"/>
-      <c r="C41" s="60" t="s">
+      <c r="B41" s="96"/>
+      <c r="C41" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="D41" s="61">
+      <c r="D41" s="60">
         <v>28</v>
       </c>
       <c r="E41" s="3"/>
@@ -2934,14 +2934,14 @@
       <c r="Z41" s="3"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A42" s="91" t="s">
+      <c r="A42" s="95" t="s">
         <v>59</v>
       </c>
-      <c r="B42" s="92"/>
-      <c r="C42" s="60" t="s">
+      <c r="B42" s="96"/>
+      <c r="C42" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="D42" s="61">
+      <c r="D42" s="60">
         <v>32</v>
       </c>
       <c r="E42" s="3"/>
@@ -2968,14 +2968,14 @@
       <c r="Z42" s="3"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A43" s="91" t="s">
+      <c r="A43" s="95" t="s">
         <v>60</v>
       </c>
-      <c r="B43" s="92"/>
-      <c r="C43" s="60" t="s">
+      <c r="B43" s="96"/>
+      <c r="C43" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="D43" s="61">
+      <c r="D43" s="60">
         <v>36</v>
       </c>
       <c r="E43" s="3"/>
@@ -3002,14 +3002,14 @@
       <c r="Z43" s="3"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A44" s="91" t="s">
+      <c r="A44" s="95" t="s">
         <v>61</v>
       </c>
-      <c r="B44" s="92"/>
-      <c r="C44" s="60" t="s">
+      <c r="B44" s="96"/>
+      <c r="C44" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="D44" s="61">
+      <c r="D44" s="60">
         <v>32</v>
       </c>
       <c r="E44" s="3"/>
@@ -3092,16 +3092,16 @@
       <c r="Z46" s="3"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A47" s="87" t="s">
+      <c r="A47" s="86" t="s">
         <v>111</v>
       </c>
-      <c r="B47" s="87" t="s">
+      <c r="B47" s="86" t="s">
         <v>112</v>
       </c>
-      <c r="C47" s="96" t="s">
+      <c r="C47" s="99" t="s">
         <v>113</v>
       </c>
-      <c r="D47" s="96"/>
+      <c r="D47" s="99"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -3126,16 +3126,16 @@
       <c r="Z47" s="3"/>
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A48" s="88">
+      <c r="A48" s="87">
         <v>44508</v>
       </c>
-      <c r="B48" s="89">
+      <c r="B48" s="88">
         <v>1</v>
       </c>
-      <c r="C48" s="97" t="s">
+      <c r="C48" s="100" t="s">
         <v>115</v>
       </c>
-      <c r="D48" s="98"/>
+      <c r="D48" s="101"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
@@ -3160,16 +3160,16 @@
       <c r="Z48" s="3"/>
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A49" s="88">
+      <c r="A49" s="87">
         <v>44512</v>
       </c>
-      <c r="B49" s="89">
+      <c r="B49" s="88">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C49" s="97" t="s">
+      <c r="C49" s="100" t="s">
         <v>116</v>
       </c>
-      <c r="D49" s="98"/>
+      <c r="D49" s="101"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
@@ -29963,16 +29963,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
     <mergeCell ref="A11:I11"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -30000,62 +30000,62 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="61" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="61" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="61" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="61" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="62" t="s">
+      <c r="A8" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="61" t="s">
         <v>73</v>
       </c>
     </row>
@@ -31068,7 +31068,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
@@ -31167,7 +31167,7 @@
         <v>78</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="63" t="s">
+      <c r="C8" s="62" t="s">
         <v>79</v>
       </c>
       <c r="D8" s="2"/>
@@ -31189,103 +31189,103 @@
       <c r="I9" s="9"/>
     </row>
     <row r="10" spans="1:26" ht="30">
-      <c r="A10" s="64" t="s">
+      <c r="A10" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="65" t="s">
+      <c r="C10" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="65" t="s">
+      <c r="D10" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="65" t="s">
+      <c r="E10" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="65" t="s">
+      <c r="F10" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="65" t="s">
+      <c r="G10" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="65" t="s">
+      <c r="H10" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="65" t="s">
+      <c r="I10" s="64" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:26">
-      <c r="A11" s="104" t="s">
+      <c r="A11" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="100"/>
-      <c r="C11" s="100"/>
-      <c r="D11" s="100"/>
-      <c r="E11" s="100"/>
-      <c r="F11" s="100"/>
-      <c r="G11" s="100"/>
-      <c r="H11" s="100"/>
-      <c r="I11" s="101"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="91"/>
+      <c r="D11" s="91"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="91"/>
+      <c r="G11" s="91"/>
+      <c r="H11" s="91"/>
+      <c r="I11" s="92"/>
       <c r="K11" s="12"/>
     </row>
     <row r="12" spans="1:26" ht="17.25" customHeight="1">
-      <c r="A12" s="66" t="s">
+      <c r="A12" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="68" t="s">
+      <c r="C12" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="69" t="s">
+      <c r="D12" s="68" t="s">
         <v>80</v>
       </c>
-      <c r="E12" s="69" t="s">
+      <c r="E12" s="68" t="s">
         <v>81</v>
       </c>
-      <c r="F12" s="70">
+      <c r="F12" s="69">
         <v>44368</v>
       </c>
-      <c r="G12" s="70">
+      <c r="G12" s="69">
         <v>44370</v>
       </c>
-      <c r="H12" s="71">
+      <c r="H12" s="70">
         <v>6</v>
       </c>
-      <c r="I12" s="72" t="s">
+      <c r="I12" s="71" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="17.25" customHeight="1">
-      <c r="A13" s="73" t="s">
+      <c r="A13" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="74" t="s">
+      <c r="B13" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="74" t="s">
+      <c r="C13" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="72" t="s">
+      <c r="D13" s="71" t="s">
         <v>83</v>
       </c>
-      <c r="E13" s="75" t="s">
+      <c r="E13" s="74" t="s">
         <v>84</v>
       </c>
-      <c r="F13" s="76">
+      <c r="F13" s="75">
         <v>44375</v>
       </c>
-      <c r="G13" s="76">
+      <c r="G13" s="75">
         <v>44377</v>
       </c>
-      <c r="H13" s="74">
+      <c r="H13" s="73">
         <v>4</v>
       </c>
-      <c r="I13" s="72" t="s">
+      <c r="I13" s="71" t="s">
         <v>82</v>
       </c>
       <c r="J13" s="22"/>
@@ -31307,334 +31307,334 @@
       <c r="Z13" s="22"/>
     </row>
     <row r="14" spans="1:26" ht="17.25" customHeight="1">
-      <c r="A14" s="77" t="s">
+      <c r="A14" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="67" t="s">
+      <c r="B14" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="68" t="s">
+      <c r="C14" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="69" t="s">
+      <c r="D14" s="68" t="s">
         <v>85</v>
       </c>
-      <c r="E14" s="69" t="s">
+      <c r="E14" s="68" t="s">
         <v>84</v>
       </c>
-      <c r="F14" s="70">
+      <c r="F14" s="69">
         <v>44377</v>
       </c>
-      <c r="G14" s="70">
+      <c r="G14" s="69">
         <v>44380</v>
       </c>
-      <c r="H14" s="67">
+      <c r="H14" s="66">
         <v>10</v>
       </c>
-      <c r="I14" s="72" t="s">
+      <c r="I14" s="71" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="17.25" customHeight="1">
-      <c r="A15" s="66" t="s">
+      <c r="A15" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="68" t="s">
+      <c r="B15" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="68" t="s">
+      <c r="C15" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="72" t="s">
+      <c r="D15" s="71" t="s">
         <v>83</v>
       </c>
-      <c r="E15" s="72" t="s">
+      <c r="E15" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="F15" s="78">
+      <c r="F15" s="77">
         <v>44370</v>
       </c>
-      <c r="G15" s="78">
+      <c r="G15" s="77">
         <v>44372</v>
       </c>
-      <c r="H15" s="68">
+      <c r="H15" s="67">
         <v>9</v>
       </c>
-      <c r="I15" s="72" t="s">
+      <c r="I15" s="71" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="17.25" customHeight="1">
-      <c r="A16" s="77" t="s">
+      <c r="A16" s="76" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="67" t="s">
+      <c r="B16" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="67" t="s">
+      <c r="C16" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="69" t="s">
+      <c r="D16" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="E16" s="69" t="s">
+      <c r="E16" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="F16" s="70">
+      <c r="F16" s="69">
         <v>44372</v>
       </c>
-      <c r="G16" s="70">
+      <c r="G16" s="69">
         <v>44375</v>
       </c>
-      <c r="H16" s="67">
+      <c r="H16" s="66">
         <v>10</v>
       </c>
-      <c r="I16" s="72" t="s">
+      <c r="I16" s="71" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="17.25" customHeight="1">
-      <c r="A17" s="79" t="s">
+      <c r="A17" s="78" t="s">
         <v>73</v>
       </c>
-      <c r="B17" s="71" t="s">
+      <c r="B17" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="67" t="s">
+      <c r="C17" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="69" t="s">
+      <c r="D17" s="68" t="s">
         <v>83</v>
       </c>
-      <c r="E17" s="80" t="s">
+      <c r="E17" s="79" t="s">
         <v>91</v>
       </c>
-      <c r="F17" s="70">
+      <c r="F17" s="69">
         <v>44383</v>
       </c>
-      <c r="G17" s="70">
+      <c r="G17" s="69">
         <v>44386</v>
       </c>
-      <c r="H17" s="71">
+      <c r="H17" s="70">
         <v>6</v>
       </c>
-      <c r="I17" s="72" t="s">
+      <c r="I17" s="71" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="17.25" customHeight="1">
-      <c r="A18" s="104" t="s">
+      <c r="A18" s="103" t="s">
         <v>92</v>
       </c>
-      <c r="B18" s="100"/>
-      <c r="C18" s="100"/>
-      <c r="D18" s="100"/>
-      <c r="E18" s="100"/>
-      <c r="F18" s="100"/>
-      <c r="G18" s="100"/>
-      <c r="H18" s="100"/>
-      <c r="I18" s="101"/>
+      <c r="B18" s="91"/>
+      <c r="C18" s="91"/>
+      <c r="D18" s="91"/>
+      <c r="E18" s="91"/>
+      <c r="F18" s="91"/>
+      <c r="G18" s="91"/>
+      <c r="H18" s="91"/>
+      <c r="I18" s="92"/>
     </row>
     <row r="19" spans="1:9" ht="17.25" customHeight="1">
-      <c r="A19" s="79" t="s">
+      <c r="A19" s="78" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="71" t="s">
+      <c r="B19" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="67" t="s">
+      <c r="C19" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="D19" s="69" t="s">
+      <c r="D19" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="80" t="s">
+      <c r="E19" s="79" t="s">
         <v>91</v>
       </c>
-      <c r="F19" s="81">
+      <c r="F19" s="80">
         <v>44397</v>
       </c>
-      <c r="G19" s="81">
+      <c r="G19" s="80">
         <v>44399</v>
       </c>
-      <c r="H19" s="71">
+      <c r="H19" s="70">
         <v>10</v>
       </c>
-      <c r="I19" s="72" t="s">
+      <c r="I19" s="71" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="17.25" customHeight="1">
-      <c r="A20" s="77" t="s">
+      <c r="A20" s="76" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="67" t="s">
+      <c r="B20" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="C20" s="67" t="s">
+      <c r="C20" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="D20" s="69" t="s">
+      <c r="D20" s="68" t="s">
         <v>83</v>
       </c>
-      <c r="E20" s="82" t="s">
+      <c r="E20" s="81" t="s">
         <v>96</v>
       </c>
-      <c r="F20" s="78">
+      <c r="F20" s="77">
         <v>44407</v>
       </c>
-      <c r="G20" s="78">
+      <c r="G20" s="77">
         <v>44410</v>
       </c>
-      <c r="H20" s="67">
+      <c r="H20" s="66">
         <v>6</v>
       </c>
-      <c r="I20" s="72" t="s">
+      <c r="I20" s="71" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="17.25" customHeight="1">
-      <c r="A21" s="77" t="s">
+      <c r="A21" s="76" t="s">
         <v>69</v>
       </c>
-      <c r="B21" s="67" t="s">
+      <c r="B21" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="67" t="s">
+      <c r="C21" s="66" t="s">
         <v>97</v>
       </c>
-      <c r="D21" s="69" t="s">
+      <c r="D21" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="E21" s="82" t="s">
+      <c r="E21" s="81" t="s">
         <v>96</v>
       </c>
-      <c r="F21" s="78">
+      <c r="F21" s="77">
         <v>44410</v>
       </c>
-      <c r="G21" s="78">
+      <c r="G21" s="77">
         <v>44413</v>
       </c>
-      <c r="H21" s="67">
+      <c r="H21" s="66">
         <v>10</v>
       </c>
-      <c r="I21" s="72" t="s">
+      <c r="I21" s="71" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="17.25" customHeight="1">
-      <c r="A22" s="77" t="s">
+      <c r="A22" s="76" t="s">
         <v>71</v>
       </c>
-      <c r="B22" s="67" t="s">
+      <c r="B22" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="C22" s="67" t="s">
+      <c r="C22" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="D22" s="69" t="s">
+      <c r="D22" s="68" t="s">
         <v>83</v>
       </c>
-      <c r="E22" s="69" t="s">
+      <c r="E22" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="F22" s="78">
+      <c r="F22" s="77">
         <v>44415</v>
       </c>
-      <c r="G22" s="78">
+      <c r="G22" s="77">
         <v>44418</v>
       </c>
-      <c r="H22" s="67">
+      <c r="H22" s="66">
         <v>6</v>
       </c>
-      <c r="I22" s="72" t="s">
+      <c r="I22" s="71" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="17.25" customHeight="1">
-      <c r="A23" s="77" t="s">
+      <c r="A23" s="76" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="67" t="s">
+      <c r="B23" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="67" t="s">
+      <c r="C23" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="D23" s="69" t="s">
+      <c r="D23" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="E23" s="69" t="s">
+      <c r="E23" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="F23" s="78">
+      <c r="F23" s="77">
         <v>44418</v>
       </c>
-      <c r="G23" s="78">
+      <c r="G23" s="77">
         <v>44422</v>
       </c>
-      <c r="H23" s="67">
+      <c r="H23" s="66">
         <v>10</v>
       </c>
-      <c r="I23" s="72" t="s">
+      <c r="I23" s="71" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="17.25" customHeight="1">
-      <c r="A24" s="77" t="s">
+      <c r="A24" s="76" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="67" t="s">
+      <c r="B24" s="66" t="s">
         <v>101</v>
       </c>
-      <c r="C24" s="67" t="s">
+      <c r="C24" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="D24" s="69" t="s">
+      <c r="D24" s="68" t="s">
         <v>83</v>
       </c>
-      <c r="E24" s="69" t="s">
+      <c r="E24" s="68" t="s">
         <v>103</v>
       </c>
-      <c r="F24" s="78">
+      <c r="F24" s="77">
         <v>44424</v>
       </c>
-      <c r="G24" s="78">
+      <c r="G24" s="77">
         <v>44427</v>
       </c>
-      <c r="H24" s="67">
+      <c r="H24" s="66">
         <v>6</v>
       </c>
-      <c r="I24" s="72" t="s">
+      <c r="I24" s="71" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="17.25" customHeight="1">
-      <c r="A25" s="77" t="s">
+      <c r="A25" s="76" t="s">
         <v>66</v>
       </c>
-      <c r="B25" s="67" t="s">
+      <c r="B25" s="66" t="s">
         <v>101</v>
       </c>
-      <c r="C25" s="67" t="s">
+      <c r="C25" s="66" t="s">
         <v>104</v>
       </c>
-      <c r="D25" s="69" t="s">
+      <c r="D25" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="E25" s="69" t="s">
+      <c r="E25" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="F25" s="78">
+      <c r="F25" s="77">
         <v>44427</v>
       </c>
-      <c r="G25" s="78">
+      <c r="G25" s="77">
         <v>44430</v>
       </c>
-      <c r="H25" s="67">
+      <c r="H25" s="66">
         <v>10</v>
       </c>
-      <c r="I25" s="72" t="s">
+      <c r="I25" s="71" t="s">
         <v>82</v>
       </c>
     </row>
@@ -31653,93 +31653,93 @@
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1"/>
     <row r="28" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A28" s="105" t="s">
+      <c r="A28" s="104" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="106"/>
-      <c r="C28" s="92"/>
+      <c r="B28" s="105"/>
+      <c r="C28" s="96"/>
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A29" s="107" t="s">
+      <c r="A29" s="106" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="92"/>
-      <c r="C29" s="58" t="s">
+      <c r="B29" s="96"/>
+      <c r="C29" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="59" t="s">
+      <c r="D29" s="58" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A30" s="103" t="s">
+      <c r="A30" s="102" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="92"/>
-      <c r="C30" s="83" t="s">
+      <c r="B30" s="96"/>
+      <c r="C30" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="84">
+      <c r="D30" s="83">
         <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A31" s="103" t="s">
+      <c r="A31" s="102" t="s">
         <v>106</v>
       </c>
-      <c r="B31" s="92"/>
-      <c r="C31" s="83" t="s">
+      <c r="B31" s="96"/>
+      <c r="C31" s="82" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="59">
+      <c r="D31" s="58">
         <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A32" s="103" t="s">
+      <c r="A32" s="102" t="s">
         <v>107</v>
       </c>
-      <c r="B32" s="92"/>
-      <c r="C32" s="83" t="s">
+      <c r="B32" s="96"/>
+      <c r="C32" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="D32" s="59">
+      <c r="D32" s="58">
         <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A33" s="103" t="s">
+      <c r="A33" s="102" t="s">
         <v>108</v>
       </c>
-      <c r="B33" s="92"/>
-      <c r="C33" s="83" t="s">
+      <c r="B33" s="96"/>
+      <c r="C33" s="82" t="s">
         <v>69</v>
       </c>
-      <c r="D33" s="84">
+      <c r="D33" s="83">
         <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A34" s="103" t="s">
+      <c r="A34" s="102" t="s">
         <v>109</v>
       </c>
-      <c r="B34" s="92"/>
-      <c r="C34" s="83" t="s">
+      <c r="B34" s="96"/>
+      <c r="C34" s="82" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="84">
+      <c r="D34" s="83">
         <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A35" s="103" t="s">
+      <c r="A35" s="102" t="s">
         <v>110</v>
       </c>
-      <c r="B35" s="92"/>
-      <c r="C35" s="83" t="s">
+      <c r="B35" s="96"/>
+      <c r="C35" s="82" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="84">
+      <c r="D35" s="83">
         <v>20</v>
       </c>
     </row>

</xml_diff>